<commit_message>
Cambio de nombre bases
</commit_message>
<xml_diff>
--- a/Bases/GDP_countries_corregida.xlsx
+++ b/Bases/GDP_countries_corregida.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e8b1635bbae8cdf/Documents/Codigo_compartido_Melo/Climate_Change_and_Financial_Stability/Climate-Change-and-Financial-Stability/Bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{764BB59C-CA9A-4F68-8C60-5EE9389B639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7386D24-D4A0-4383-A0F3-1694F73BEA9E}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{764BB59C-CA9A-4F68-8C60-5EE9389B639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C41A657A-BF0B-4431-8B11-2734E8FFE364}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1B6FECDE-2716-47F5-9347-D5C4059D6B3D}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1B6FECDE-2716-47F5-9347-D5C4059D6B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEF8FF5-A0BC-4AED-AB3D-E37A9816DD73}">
   <dimension ref="A1:AB77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="K81" sqref="K78:K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +874,7 @@
         <v>600282.03406460001</v>
       </c>
       <c r="K2" s="1">
-        <v>300726.7</v>
+        <v>300386.48622321233</v>
       </c>
       <c r="L2" s="1">
         <v>9039056.4649918061</v>
@@ -899,7 +895,7 @@
         <v>249544.31936885</v>
       </c>
       <c r="R2" s="1">
-        <v>6782815.7800000003</v>
+        <v>7862150.8366930299</v>
       </c>
       <c r="S2" s="1">
         <v>554176.42698659655</v>
@@ -964,7 +960,7 @@
         <v>600003.22952306992</v>
       </c>
       <c r="K3" s="1">
-        <v>300843.87</v>
+        <v>299951.95270165417</v>
       </c>
       <c r="L3" s="1">
         <v>9227139.5361973885</v>
@@ -985,7 +981,7 @@
         <v>248811.53950478</v>
       </c>
       <c r="R3" s="1">
-        <v>6904071.5599999996</v>
+        <v>8002701.7958599422</v>
       </c>
       <c r="S3" s="1">
         <v>556945.60899617919</v>
@@ -1050,7 +1046,7 @@
         <v>598748.56762618001</v>
       </c>
       <c r="K4" s="1">
-        <v>298718.76</v>
+        <v>299721.9960238738</v>
       </c>
       <c r="L4" s="1">
         <v>9341277.7434220091</v>
@@ -1071,7 +1067,7 @@
         <v>250005.87491324</v>
       </c>
       <c r="R4" s="1">
-        <v>7079086.1399999997</v>
+        <v>8205566.0732096778</v>
       </c>
       <c r="S4" s="1">
         <v>558425.74074034055</v>
@@ -1136,7 +1132,7 @@
         <v>598260.62973517005</v>
       </c>
       <c r="K5" s="1">
-        <v>297933.31</v>
+        <v>297914.64420854329</v>
       </c>
       <c r="L5" s="1">
         <v>9555763.2139140517</v>
@@ -1157,7 +1153,7 @@
         <v>250040.37070432998</v>
       </c>
       <c r="R5" s="1">
-        <v>7043018.54</v>
+        <v>8163759.1143771298</v>
       </c>
       <c r="S5" s="1">
         <v>562721.80601886159</v>
@@ -1222,7 +1218,7 @@
         <v>595193.70607165003</v>
       </c>
       <c r="K6" s="1">
-        <v>298841.43</v>
+        <v>298126.1428252309</v>
       </c>
       <c r="L6" s="1">
         <v>9632883.6242009569</v>
@@ -1243,7 +1239,7 @@
         <v>251724.24880842998</v>
       </c>
       <c r="R6" s="1">
-        <v>7073611.1200000001</v>
+        <v>8199219.8259713296</v>
       </c>
       <c r="S6" s="1">
         <v>568833.0300044677</v>
@@ -1308,7 +1304,7 @@
         <v>597772.70105749997</v>
       </c>
       <c r="K7" s="1">
-        <v>302711.39</v>
+        <v>302689.12934453133</v>
       </c>
       <c r="L7" s="1">
         <v>9692946.8143302854</v>
@@ -1329,7 +1325,7 @@
         <v>253478.14128097001</v>
       </c>
       <c r="R7" s="1">
-        <v>7199434.2699999996</v>
+        <v>8345064.951969848</v>
       </c>
       <c r="S7" s="1">
         <v>576050.6811118311</v>
@@ -1394,7 +1390,7 @@
         <v>600560.84781946999</v>
       </c>
       <c r="K8" s="1">
-        <v>306121.42</v>
+        <v>307446.6945911845</v>
       </c>
       <c r="L8" s="1">
         <v>9750560.2973093297</v>
@@ -1415,7 +1411,7 @@
         <v>255869.41555382</v>
       </c>
       <c r="R8" s="1">
-        <v>7385975.1900000004</v>
+        <v>8561289.7296271101</v>
       </c>
       <c r="S8" s="1">
         <v>582570.59646946751</v>
@@ -1480,7 +1476,7 @@
         <v>599794.14224024001</v>
       </c>
       <c r="K9" s="1">
-        <v>309677.15999999997</v>
+        <v>309559.37350042415</v>
       </c>
       <c r="L9" s="1">
         <v>9758181.6084435694</v>
@@ -1501,7 +1497,7 @@
         <v>257224.14244376001</v>
       </c>
       <c r="R9" s="1">
-        <v>7467978</v>
+        <v>8656341.4725748617</v>
       </c>
       <c r="S9" s="1">
         <v>587417.53004323342</v>
@@ -1566,7 +1562,7 @@
         <v>590924.51671189</v>
       </c>
       <c r="K10" s="1">
-        <v>309750.73</v>
+        <v>309304.80607452011</v>
       </c>
       <c r="L10" s="1">
         <v>9977838.6829195544</v>
@@ -1587,7 +1583,7 @@
         <v>258234.00440338001</v>
       </c>
       <c r="R10" s="1">
-        <v>7647009.7999999998</v>
+        <v>8863862.2225052826</v>
       </c>
       <c r="S10" s="1">
         <v>591146.27172009216</v>
@@ -1652,7 +1648,7 @@
         <v>591551.82462701004</v>
       </c>
       <c r="K11" s="1">
-        <v>301536.62</v>
+        <v>301783.14617922954</v>
       </c>
       <c r="L11" s="1">
         <v>10230612.168871678</v>
@@ -1673,7 +1669,7 @@
         <v>262559.83239428001</v>
       </c>
       <c r="R11" s="1">
-        <v>7732307.3200000003</v>
+        <v>8962732.9509561434</v>
       </c>
       <c r="S11" s="1">
         <v>594033.25526908261</v>
@@ -1738,7 +1734,7 @@
         <v>596082.37769697001</v>
       </c>
       <c r="K12" s="1">
-        <v>319134.87</v>
+        <v>320295.04328348767</v>
       </c>
       <c r="L12" s="1">
         <v>10499807.765720204</v>
@@ -1759,7 +1755,7 @@
         <v>265936.32877596997</v>
       </c>
       <c r="R12" s="1">
-        <v>7862841.5899999999</v>
+        <v>9114038.8630243372</v>
       </c>
       <c r="S12" s="1">
         <v>597256.9574480115</v>
@@ -1824,7 +1820,7 @@
         <v>597755.19573286001</v>
       </c>
       <c r="K13" s="1">
-        <v>323984.13</v>
+        <v>323659.79400351795</v>
       </c>
       <c r="L13" s="1">
         <v>10844581.364649897</v>
@@ -1845,7 +1841,7 @@
         <v>267978.46101232996</v>
       </c>
       <c r="R13" s="1">
-        <v>8006245.5800000001</v>
+        <v>9280262.424406426</v>
       </c>
       <c r="S13" s="1">
         <v>600702.72936963476</v>
@@ -1910,7 +1906,7 @@
         <v>596709.79617204005</v>
       </c>
       <c r="K14" s="1">
-        <v>333262.58</v>
+        <v>332905.74443922174</v>
       </c>
       <c r="L14" s="1">
         <v>10884139.598632354</v>
@@ -1931,7 +1927,7 @@
         <v>273986.12153482001</v>
       </c>
       <c r="R14" s="1">
-        <v>8156656.2599999998</v>
+        <v>9454607.6334127299</v>
       </c>
       <c r="S14" s="1">
         <v>609796.05472684558</v>
@@ -1996,7 +1992,7 @@
         <v>599776.64612893004</v>
       </c>
       <c r="K15" s="1">
-        <v>338482.6</v>
+        <v>338913.07423902903</v>
       </c>
       <c r="L15" s="1">
         <v>11142991.987512982</v>
@@ -2017,7 +2013,7 @@
         <v>276295.94482924999</v>
       </c>
       <c r="R15" s="1">
-        <v>8313850.04</v>
+        <v>9636815.3269280549</v>
       </c>
       <c r="S15" s="1">
         <v>618317.67352694657</v>
@@ -2082,7 +2078,7 @@
         <v>598522.06715200003</v>
       </c>
       <c r="K16" s="1">
-        <v>341734.7</v>
+        <v>342769.27083565341</v>
       </c>
       <c r="L16" s="1">
         <v>11410100.796789026</v>
@@ -2103,7 +2099,7 @@
         <v>276181.76469054999</v>
       </c>
       <c r="R16" s="1">
-        <v>8439766.2400000002</v>
+        <v>9782768.3046526536</v>
       </c>
       <c r="S16" s="1">
         <v>628427.92144203186</v>
@@ -2168,7 +2164,7 @@
         <v>597964.42121561</v>
       </c>
       <c r="K17" s="1">
-        <v>350250.39</v>
+        <v>349644.12950681936</v>
       </c>
       <c r="L17" s="1">
         <v>11631118.819681857</v>
@@ -2189,7 +2185,7 @@
         <v>279022.04213096999</v>
       </c>
       <c r="R17" s="1">
-        <v>8534137.2300000004</v>
+        <v>9892156.3561910335</v>
       </c>
       <c r="S17" s="1">
         <v>635139.07206631696</v>
@@ -2254,7 +2250,7 @@
         <v>597981.86204694991</v>
       </c>
       <c r="K18" s="1">
-        <v>353745.29</v>
+        <v>353412.65031325334</v>
       </c>
       <c r="L18" s="1">
         <v>11834716.702839268</v>
@@ -2275,7 +2271,7 @@
         <v>280982.72338890994</v>
       </c>
       <c r="R18" s="1">
-        <v>8683320.9299999997</v>
+        <v>10065079.334768439</v>
       </c>
       <c r="S18" s="1">
         <v>641595.85748671251</v>
@@ -2340,7 +2336,7 @@
         <v>601188.18337458</v>
       </c>
       <c r="K19" s="1">
-        <v>364061.59</v>
+        <v>364455.95444786246</v>
       </c>
       <c r="L19" s="1">
         <v>12209521.896833621</v>
@@ -2361,7 +2357,7 @@
         <v>282270.69023033004</v>
       </c>
       <c r="R19" s="1">
-        <v>8815506.7300000004</v>
+        <v>10218299.583180772</v>
       </c>
       <c r="S19" s="1">
         <v>653109.65076655266</v>
@@ -2426,7 +2422,7 @@
         <v>606276.49294087</v>
       </c>
       <c r="K20" s="1">
-        <v>370520.24</v>
+        <v>371341.58032133244</v>
       </c>
       <c r="L20" s="1">
         <v>12379458.989148173</v>
@@ -2447,7 +2443,7 @@
         <v>287633.99540983001</v>
       </c>
       <c r="R20" s="1">
-        <v>8970854.0299999993</v>
+        <v>10398366.964302361</v>
       </c>
       <c r="S20" s="1">
         <v>662015.58555487671</v>
@@ -2512,7 +2508,7 @@
         <v>609134.32010822999</v>
       </c>
       <c r="K21" s="1">
-        <v>375890.25</v>
+        <v>375814.58379280585</v>
       </c>
       <c r="L21" s="1">
         <v>12692386.395124095</v>
@@ -2533,7 +2529,7 @@
         <v>292652.34267844999</v>
       </c>
       <c r="R21" s="1">
-        <v>9155908.4000000004</v>
+        <v>10612868.649332881</v>
       </c>
       <c r="S21" s="1">
         <v>666446.83040668664</v>
@@ -2598,7 +2594,7 @@
         <v>614989.39053372003</v>
       </c>
       <c r="K22" s="1">
-        <v>384550.40000000002</v>
+        <v>384123.01854217437</v>
       </c>
       <c r="L22" s="1">
         <v>13010394.675189495</v>
@@ -2619,7 +2615,7 @@
         <v>297132.98331670003</v>
       </c>
       <c r="R22" s="1">
-        <v>9332672.8800000008</v>
+        <v>10817761.285526885</v>
       </c>
       <c r="S22" s="1">
         <v>678157.39531795296</v>
@@ -2684,7 +2680,7 @@
         <v>625584.23029859993</v>
       </c>
       <c r="K23" s="1">
-        <v>387429.82</v>
+        <v>387993.82777049736</v>
       </c>
       <c r="L23" s="1">
         <v>13197298.257767171</v>
@@ -2705,7 +2701,7 @@
         <v>304025.07501125999</v>
       </c>
       <c r="R23" s="1">
-        <v>9512336.5299999993</v>
+        <v>11026014.428781707</v>
       </c>
       <c r="S23" s="1">
         <v>687788.90146779723</v>
@@ -2770,7 +2766,7 @@
         <v>630463.43415541004</v>
       </c>
       <c r="K24" s="1">
-        <v>394547.89</v>
+        <v>394881.76090160385</v>
       </c>
       <c r="L24" s="1">
         <v>13633164.670729868</v>
@@ -2791,7 +2787,7 @@
         <v>308887.21492400003</v>
       </c>
       <c r="R24" s="1">
-        <v>9730752.0500000007</v>
+        <v>11279185.948633293</v>
       </c>
       <c r="S24" s="1">
         <v>697288.30380256148</v>
@@ -2856,7 +2852,7 @@
         <v>640012.76379952999</v>
       </c>
       <c r="K25" s="1">
-        <v>400957.37</v>
+        <v>401055.21325124567</v>
       </c>
       <c r="L25" s="1">
         <v>13866431.229374129</v>
@@ -2877,7 +2873,7 @@
         <v>304451.85582284996</v>
       </c>
       <c r="R25" s="1">
-        <v>9915562.4600000009</v>
+        <v>11493404.84693131</v>
       </c>
       <c r="S25" s="1">
         <v>706930.57510613708</v>
@@ -2942,7 +2938,7 @@
         <v>640413.70022707991</v>
       </c>
       <c r="K26" s="1">
-        <v>406135.86</v>
+        <v>406471.11601020646</v>
       </c>
       <c r="L26" s="1">
         <v>14253847.878697747</v>
@@ -2963,7 +2959,7 @@
         <v>318034.45733844</v>
       </c>
       <c r="R26" s="1">
-        <v>10095396.15</v>
+        <v>11701855.085888594</v>
       </c>
       <c r="S26" s="1">
         <v>718408.76648470724</v>
@@ -3028,7 +3024,7 @@
         <v>645780.70377496001</v>
       </c>
       <c r="K27" s="1">
-        <v>412299.96</v>
+        <v>413105.25080128794</v>
       </c>
       <c r="L27" s="1">
         <v>14613047.530845812</v>
@@ -3049,7 +3045,7 @@
         <v>322293.06037798</v>
       </c>
       <c r="R27" s="1">
-        <v>10350183.560000001</v>
+        <v>11997186.275843298</v>
       </c>
       <c r="S27" s="1">
         <v>724296.53663642413</v>
@@ -3114,7 +3110,7 @@
         <v>649126.35827338998</v>
       </c>
       <c r="K28" s="1">
-        <v>421494.89</v>
+        <v>421144.50549305405</v>
       </c>
       <c r="L28" s="1">
         <v>14875256.92582128</v>
@@ -3135,7 +3131,7 @@
         <v>327895.41860032</v>
       </c>
       <c r="R28" s="1">
-        <v>10578416.529999999</v>
+        <v>12261737.475814812</v>
       </c>
       <c r="S28" s="1">
         <v>732784.86035391118</v>
@@ -3200,7 +3196,7 @@
         <v>653308.44482307998</v>
       </c>
       <c r="K29" s="1">
-        <v>428800.97</v>
+        <v>428704.61968228786</v>
       </c>
       <c r="L29" s="1">
         <v>15377537.621525152</v>
@@ -3221,7 +3217,7 @@
         <v>332223.47812488</v>
       </c>
       <c r="R29" s="1">
-        <v>10916273.43</v>
+        <v>12653356.819843849</v>
       </c>
       <c r="S29" s="1">
         <v>743169.00453751523</v>
@@ -3286,7 +3282,7 @@
         <v>657490.62350605009</v>
       </c>
       <c r="K30" s="1">
-        <v>433757.64</v>
+        <v>434559.67047807999</v>
       </c>
       <c r="L30" s="1">
         <v>15470717.223130617</v>
@@ -3307,7 +3303,7 @@
         <v>336830.57233692997</v>
       </c>
       <c r="R30" s="1">
-        <v>11205900.91</v>
+        <v>12989072.108558824</v>
       </c>
       <c r="S30" s="1">
         <v>746290.36086203682</v>
@@ -3372,7 +3368,7 @@
         <v>655887.51351555006</v>
       </c>
       <c r="K31" s="1">
-        <v>428876.67</v>
+        <v>429483.70367757714</v>
       </c>
       <c r="L31" s="1">
         <v>15632216.435260851</v>
@@ -3393,7 +3389,7 @@
         <v>338842.95079120999</v>
       </c>
       <c r="R31" s="1">
-        <v>11275557.01</v>
+        <v>13069812.439077783</v>
       </c>
       <c r="S31" s="1">
         <v>755401.67940477107</v>
@@ -3458,7 +3454,7 @@
         <v>651705.41775253008</v>
       </c>
       <c r="K32" s="1">
-        <v>425939.99</v>
+        <v>424702.29676867917</v>
       </c>
       <c r="L32" s="1">
         <v>15768311.276943617</v>
@@ -3479,7 +3475,7 @@
         <v>338934.62963221996</v>
       </c>
       <c r="R32" s="1">
-        <v>11107475.83</v>
+        <v>12874984.857201563</v>
       </c>
       <c r="S32" s="1">
         <v>757206.61121581018</v>
@@ -3544,7 +3540,7 @@
         <v>641319.92324368004</v>
       </c>
       <c r="K33" s="1">
-        <v>417306.66</v>
+        <v>416203.12872135232</v>
       </c>
       <c r="L33" s="1">
         <v>15787636.744462578</v>
@@ -3565,7 +3561,7 @@
         <v>339385.95731402002</v>
       </c>
       <c r="R33" s="1">
-        <v>10746237.25</v>
+        <v>12456263.144061955</v>
       </c>
       <c r="S33" s="1">
         <v>752896.24366161635</v>
@@ -3630,7 +3626,7 @@
         <v>611277.81947035994</v>
       </c>
       <c r="K34" s="1">
-        <v>400055.94</v>
+        <v>401918.89669321</v>
       </c>
       <c r="L34" s="1">
         <v>15496121.593578078</v>
@@ -3651,7 +3647,7 @@
         <v>344199.09646690998</v>
       </c>
       <c r="R34" s="1">
-        <v>10367219.43</v>
+        <v>12016933.023204124</v>
       </c>
       <c r="S34" s="1">
         <v>741184.6022349766</v>
@@ -3716,7 +3712,7 @@
         <v>612253.61233241006</v>
       </c>
       <c r="K35" s="1">
-        <v>415814.11</v>
+        <v>416210.05049426219</v>
       </c>
       <c r="L35" s="1">
         <v>16395527.037312277</v>
@@ -3737,7 +3733,7 @@
         <v>344946.10235803999</v>
       </c>
       <c r="R35" s="1">
-        <v>10215976.1</v>
+        <v>11841622.665929833</v>
       </c>
       <c r="S35" s="1">
         <v>738640.79640816338</v>
@@ -3802,7 +3798,7 @@
         <v>615668.97487621999</v>
       </c>
       <c r="K36" s="1">
-        <v>419363.86</v>
+        <v>418362.72186920262</v>
       </c>
       <c r="L36" s="1">
         <v>16814245.500222947</v>
@@ -3823,7 +3819,7 @@
         <v>347424.49942402</v>
       </c>
       <c r="R36" s="1">
-        <v>10257905.039999999</v>
+        <v>11890223.666792674</v>
       </c>
       <c r="S36" s="1">
         <v>740353.7630487514</v>
@@ -3888,7 +3884,7 @@
         <v>620199.53715950996</v>
       </c>
       <c r="K37" s="1">
-        <v>427130.74</v>
+        <v>426530.41390273906</v>
       </c>
       <c r="L37" s="1">
         <v>17171812.014270805</v>
@@ -3909,7 +3905,7 @@
         <v>352681.15589091997</v>
       </c>
       <c r="R37" s="1">
-        <v>10368865.66</v>
+        <v>12018841.21614108</v>
       </c>
       <c r="S37" s="1">
         <v>745291.66217155091</v>
@@ -3974,7 +3970,7 @@
         <v>625235.71771169</v>
       </c>
       <c r="K38" s="1">
-        <v>431299.75</v>
+        <v>434541.98150286608</v>
       </c>
       <c r="L38" s="1">
         <v>17618293.82488475</v>
@@ -3995,7 +3991,7 @@
         <v>351171.89529534004</v>
       </c>
       <c r="R38" s="1">
-        <v>10590599.92</v>
+        <v>12275859.585566096</v>
       </c>
       <c r="S38" s="1">
         <v>753987.21509837417</v>
@@ -4060,7 +4056,7 @@
         <v>639315.67413240008</v>
       </c>
       <c r="K39" s="1">
-        <v>442307.12</v>
+        <v>442037.49247827532</v>
       </c>
       <c r="L39" s="1">
         <v>18041639.512412626</v>
@@ -4081,7 +4077,7 @@
         <v>356200.84234883002</v>
       </c>
       <c r="R39" s="1">
-        <v>10691221.130000001</v>
+        <v>12392492.424188629</v>
       </c>
       <c r="S39" s="1">
         <v>760316.27965913992</v>
@@ -4146,7 +4142,7 @@
         <v>644543.43664277007</v>
       </c>
       <c r="K40" s="1">
-        <v>447490.62</v>
+        <v>445874.46192792809</v>
       </c>
       <c r="L40" s="1">
         <v>18574859.102125794</v>
@@ -4167,7 +4163,7 @@
         <v>360425.22853898001</v>
       </c>
       <c r="R40" s="1">
-        <v>10747191.029999999</v>
+        <v>12457368.704017691</v>
       </c>
       <c r="S40" s="1">
         <v>767084.94696192874</v>
@@ -4232,7 +4228,7 @@
         <v>649771.17151314998</v>
       </c>
       <c r="K41" s="1">
-        <v>453807.7</v>
+        <v>453116.17456331226</v>
       </c>
       <c r="L41" s="1">
         <v>19006007.560576823</v>
@@ -4253,7 +4249,7 @@
         <v>364314.23381685</v>
       </c>
       <c r="R41" s="1">
-        <v>10882281.029999999</v>
+        <v>12613955.286227586</v>
       </c>
       <c r="S41" s="1">
         <v>774224.85828055791</v>
@@ -4318,7 +4314,7 @@
         <v>662370.03926942009</v>
       </c>
       <c r="K42" s="1">
-        <v>463539.11</v>
+        <v>465539.9878504824</v>
       </c>
       <c r="L42" s="1">
         <v>19353956.705812316</v>
@@ -4339,7 +4335,7 @@
         <v>369921.70597047999</v>
       </c>
       <c r="R42" s="1">
-        <v>11007988.619999999</v>
+        <v>12759666.454378871</v>
       </c>
       <c r="S42" s="1">
         <v>781849.43219898769</v>
@@ -4404,7 +4400,7 @@
         <v>662997.34718454001</v>
       </c>
       <c r="K43" s="1">
-        <v>465190.86</v>
+        <v>463727.25243399985</v>
       </c>
       <c r="L43" s="1">
         <v>19588493.48297907</v>
@@ -4425,7 +4421,7 @@
         <v>374498.86043931998</v>
       </c>
       <c r="R43" s="1">
-        <v>11112310.33</v>
+        <v>12880588.657893924</v>
       </c>
       <c r="S43" s="1">
         <v>786225.1596151226</v>
@@ -4490,7 +4486,7 @@
         <v>668852.27941009996</v>
       </c>
       <c r="K44" s="1">
-        <v>465451.79</v>
+        <v>464702.45332839951</v>
       </c>
       <c r="L44" s="1">
         <v>19587676.913928967</v>
@@ -4511,7 +4507,7 @@
         <v>378703.81369056</v>
       </c>
       <c r="R44" s="1">
-        <v>11240250.48</v>
+        <v>13028887.657151617</v>
       </c>
       <c r="S44" s="1">
         <v>789478.38907285919</v>
@@ -4576,7 +4572,7 @@
         <v>666691.55112319998</v>
       </c>
       <c r="K45" s="1">
-        <v>466600.85</v>
+        <v>467088.92681051471</v>
       </c>
       <c r="L45" s="1">
         <v>19906773.952727754</v>
@@ -4597,7 +4593,7 @@
         <v>381760.73585668998</v>
       </c>
       <c r="R45" s="1">
-        <v>11375997.029999999</v>
+        <v>13186235.261842478</v>
       </c>
       <c r="S45" s="1">
         <v>794879.11291217036</v>
@@ -4662,7 +4658,7 @@
         <v>668085.66596417001</v>
       </c>
       <c r="K46" s="1">
-        <v>467182.19</v>
+        <v>467928.76859023416</v>
       </c>
       <c r="L46" s="1">
         <v>20181685.532926977</v>
@@ -4683,7 +4679,7 @@
         <v>382964.27634147997</v>
       </c>
       <c r="R46" s="1">
-        <v>11554633.890000001</v>
+        <v>13393298.230791144</v>
       </c>
       <c r="S46" s="1">
         <v>799384.79111264099</v>
@@ -4748,7 +4744,7 @@
         <v>669479.62417854008</v>
       </c>
       <c r="K47" s="1">
-        <v>470695.58</v>
+        <v>470771.30999851576</v>
       </c>
       <c r="L47" s="1">
         <v>20415315.011149053</v>
@@ -4769,7 +4765,7 @@
         <v>382267.01505475002</v>
       </c>
       <c r="R47" s="1">
-        <v>11599358.84</v>
+        <v>13445140.16394414</v>
       </c>
       <c r="S47" s="1">
         <v>806057.57165326434</v>
@@ -4834,7 +4830,7 @@
         <v>671361.60320388002</v>
       </c>
       <c r="K48" s="1">
-        <v>473880.03</v>
+        <v>474402.16443263303</v>
       </c>
       <c r="L48" s="1">
         <v>20781591.595064539</v>
@@ -4855,7 +4851,7 @@
         <v>382419.59616844001</v>
       </c>
       <c r="R48" s="1">
-        <v>11659228.689999999</v>
+        <v>13514536.978111189</v>
       </c>
       <c r="S48" s="1">
         <v>809334.63823712245</v>
@@ -4920,7 +4916,7 @@
         <v>668364.45207904</v>
       </c>
       <c r="K49" s="1">
-        <v>480147.59</v>
+        <v>479599.64680199645</v>
       </c>
       <c r="L49" s="1">
         <v>21028286.178088225</v>
@@ -4941,7 +4937,7 @@
         <v>382154.50856628997</v>
       </c>
       <c r="R49" s="1">
-        <v>11667085.189999999</v>
+        <v>13523643.660909129</v>
       </c>
       <c r="S49" s="1">
         <v>813194.71478950663</v>
@@ -5006,7 +5002,7 @@
         <v>665314.95082019991</v>
       </c>
       <c r="K50" s="1">
-        <v>482980.45</v>
+        <v>483616.5823473034</v>
       </c>
       <c r="L50" s="1">
         <v>21364440.437044736</v>
@@ -5027,7 +5023,7 @@
         <v>381550.50679024</v>
       </c>
       <c r="R50" s="1">
-        <v>11753499.039999999</v>
+        <v>13623808.36824728</v>
       </c>
       <c r="S50" s="1">
         <v>819505.24790705659</v>
@@ -5092,7 +5088,7 @@
         <v>672424.60943594994</v>
       </c>
       <c r="K51" s="1">
-        <v>485988.4</v>
+        <v>485783.86635394237</v>
       </c>
       <c r="L51" s="1">
         <v>21664393.468113493</v>
@@ -5113,7 +5109,7 @@
         <v>384447.87430002005</v>
       </c>
       <c r="R51" s="1">
-        <v>11793520.949999999</v>
+        <v>13670198.882539494</v>
       </c>
       <c r="S51" s="1">
         <v>825466.22110414971</v>
@@ -5178,7 +5174,7 @@
         <v>676188.55827331007</v>
       </c>
       <c r="K52" s="1">
-        <v>488359.3</v>
+        <v>488713.31446653558</v>
       </c>
       <c r="L52" s="1">
         <v>22011253.854615618</v>
@@ -5199,7 +5195,7 @@
         <v>387279.78348922997</v>
       </c>
       <c r="R52" s="1">
-        <v>11798300.699999999</v>
+        <v>13675739.222469153</v>
       </c>
       <c r="S52" s="1">
         <v>829382.66092572198</v>
@@ -5264,7 +5260,7 @@
         <v>678140.29141067003</v>
       </c>
       <c r="K53" s="1">
-        <v>493431.33</v>
+        <v>493291.68270341353</v>
       </c>
       <c r="L53" s="1">
         <v>22495751.491006255</v>
@@ -5285,7 +5281,7 @@
         <v>389541.16390722996</v>
       </c>
       <c r="R53" s="1">
-        <v>11866418.76</v>
+        <v>13754696.761558503</v>
       </c>
       <c r="S53" s="1">
         <v>833847.66222387052</v>
@@ -5350,7 +5346,7 @@
         <v>684744.70029068005</v>
       </c>
       <c r="K54" s="1">
-        <v>497233.36</v>
+        <v>497779.2988065852</v>
       </c>
       <c r="L54" s="1">
         <v>22756418.477776125</v>
@@ -5371,7 +5367,7 @@
         <v>394451.56073527003</v>
       </c>
       <c r="R54" s="1">
-        <v>11865533.439999999</v>
+        <v>13753670.559223223</v>
       </c>
       <c r="S54" s="1">
         <v>832697.48244159389</v>
@@ -5436,7 +5432,7 @@
         <v>684744.70029068005</v>
       </c>
       <c r="K55" s="1">
-        <v>497241.34</v>
+        <v>496997.9075536594</v>
       </c>
       <c r="L55" s="1">
         <v>23277480.261632137</v>
@@ -5457,7 +5453,7 @@
         <v>398824.90179691999</v>
       </c>
       <c r="R55" s="1">
-        <v>11922679.619999999</v>
+        <v>13819910.295441385</v>
       </c>
       <c r="S55" s="1">
         <v>835983.93008798803</v>
@@ -5522,7 +5518,7 @@
         <v>688229.73402655008</v>
       </c>
       <c r="K56" s="1">
-        <v>503774.06</v>
+        <v>504311.9142616567</v>
       </c>
       <c r="L56" s="1">
         <v>23702459.087260239</v>
@@ -5543,7 +5539,7 @@
         <v>402017.29665203998</v>
       </c>
       <c r="R56" s="1">
-        <v>11884751.33</v>
+        <v>13775946.55365294</v>
       </c>
       <c r="S56" s="1">
         <v>840001.48546067439</v>
@@ -5608,7 +5604,7 @@
         <v>693805.87092390005</v>
       </c>
       <c r="K57" s="1">
-        <v>506336.43</v>
+        <v>506221.55449887621</v>
       </c>
       <c r="L57" s="1">
         <v>24066104.504236672</v>
@@ -5629,7 +5625,7 @@
         <v>405452.55675331998</v>
       </c>
       <c r="R57" s="1">
-        <v>11856787.689999999</v>
+        <v>13743533.114035251</v>
       </c>
       <c r="S57" s="1">
         <v>846291.18031636334</v>
@@ -5694,7 +5690,7 @@
         <v>690251.34104920994</v>
       </c>
       <c r="K58" s="1">
-        <v>509122.72</v>
+        <v>509434.79530077032</v>
       </c>
       <c r="L58" s="1">
         <v>24471394.942767818</v>
@@ -5715,7 +5711,7 @@
         <v>412020.33222331002</v>
       </c>
       <c r="R58" s="1">
-        <v>11736177.789999999</v>
+        <v>13603730.826910244</v>
       </c>
       <c r="S58" s="1">
         <v>852404.40354480513</v>
@@ -5780,7 +5776,7 @@
         <v>695339.50320223998</v>
       </c>
       <c r="K59" s="1">
-        <v>512714.65</v>
+        <v>512598.81460641691</v>
       </c>
       <c r="L59" s="1">
         <v>24995541.543035485</v>
@@ -5801,7 +5797,7 @@
         <v>414295.28780436999</v>
       </c>
       <c r="R59" s="1">
-        <v>11657567.98</v>
+        <v>13512612.001639124</v>
       </c>
       <c r="S59" s="1">
         <v>845207.89827512391</v>
@@ -5866,7 +5862,7 @@
         <v>698476.05199118995</v>
       </c>
       <c r="K60" s="1">
-        <v>514970.45</v>
+        <v>515363.67834093334</v>
       </c>
       <c r="L60" s="1">
         <v>25456993.786234491</v>
@@ -5887,7 +5883,7 @@
         <v>419815.35822316998</v>
       </c>
       <c r="R60" s="1">
-        <v>11680128.390000001</v>
+        <v>13538762.395973451</v>
       </c>
       <c r="S60" s="1">
         <v>849014.91799840389</v>
@@ -5952,7 +5948,7 @@
         <v>701542.92037473002</v>
       </c>
       <c r="K61" s="1">
-        <v>515966.73</v>
+        <v>515795.13551897602</v>
       </c>
       <c r="L61" s="1">
         <v>25974426.374312386</v>
@@ -5973,7 +5969,7 @@
         <v>423171.21291855001</v>
       </c>
       <c r="R61" s="1">
-        <v>11650018.01</v>
+        <v>13503860.623112094</v>
       </c>
       <c r="S61" s="1">
         <v>852695.06269556226</v>
@@ -6038,7 +6034,7 @@
         <v>707432.85403624002</v>
       </c>
       <c r="K62" s="1">
-        <v>514967.86</v>
+        <v>514350.79223846941</v>
       </c>
       <c r="L62" s="1">
         <v>26728301.067340571</v>
@@ -6059,7 +6055,7 @@
         <v>422431.92441464</v>
       </c>
       <c r="R62" s="1">
-        <v>11672159.77</v>
+        <v>13529525.751613315</v>
       </c>
       <c r="S62" s="1">
         <v>854731.82978160912</v>
@@ -6124,7 +6120,7 @@
         <v>710569.55945177004</v>
       </c>
       <c r="K63" s="1">
-        <v>522224.73</v>
+        <v>521912.44459946093</v>
       </c>
       <c r="L63" s="1">
         <v>27204360.823546812</v>
@@ -6145,7 +6141,7 @@
         <v>428600.53430203005</v>
       </c>
       <c r="R63" s="1">
-        <v>11678445.109999999</v>
+        <v>13536811.262520341</v>
       </c>
       <c r="S63" s="1">
         <v>855554.2106327595</v>
@@ -6210,7 +6206,7 @@
         <v>712381.85807171999</v>
       </c>
       <c r="K64" s="1">
-        <v>526819.93000000005</v>
+        <v>527832.86769495648</v>
       </c>
       <c r="L64" s="1">
         <v>27827765.928348407</v>
@@ -6231,7 +6227,7 @@
         <v>431053.73363381001</v>
       </c>
       <c r="R64" s="1">
-        <v>11690207.18</v>
+        <v>13550445.003067972</v>
       </c>
       <c r="S64" s="1">
         <v>855450.01932342618</v>
@@ -6296,7 +6292,7 @@
         <v>714960.94519084995</v>
       </c>
       <c r="K65" s="1">
-        <v>533398.42000000004</v>
+        <v>533762.51982099854</v>
       </c>
       <c r="L65" s="1">
         <v>28207289.07685433</v>
@@ -6317,7 +6313,7 @@
         <v>439317.19574015995</v>
       </c>
       <c r="R65" s="1">
-        <v>11786663.810000001</v>
+        <v>13662250.580332266</v>
       </c>
       <c r="S65" s="1">
         <v>856176.35962449783</v>
@@ -6382,7 +6378,7 @@
         <v>723569.40048891003</v>
       </c>
       <c r="K66" s="1">
-        <v>536966.59</v>
+        <v>536914.23375258339</v>
       </c>
       <c r="L66" s="1">
         <v>28432843.59446989</v>
@@ -6403,7 +6399,7 @@
         <v>444632.05804322998</v>
       </c>
       <c r="R66" s="1">
-        <v>11810435.74</v>
+        <v>13689805.281546684</v>
       </c>
       <c r="S66" s="1">
         <v>860218.59795681597</v>
@@ -6468,7 +6464,7 @@
         <v>729703.10040268989</v>
       </c>
       <c r="K67" s="1">
-        <v>542757.63</v>
+        <v>541811.77262918965</v>
       </c>
       <c r="L67" s="1">
         <v>29018142.143600341</v>
@@ -6489,7 +6485,7 @@
         <v>449006.23593001004</v>
       </c>
       <c r="R67" s="1">
-        <v>11891981.6</v>
+        <v>13784327.364392336</v>
       </c>
       <c r="S67" s="1">
         <v>864909.43680147117</v>
@@ -6554,7 +6550,7 @@
         <v>735070.15001721994</v>
       </c>
       <c r="K68" s="1">
-        <v>545434.24</v>
+        <v>546352.45565800322</v>
       </c>
       <c r="L68" s="1">
         <v>29496379.417273611</v>
@@ -6575,7 +6571,7 @@
         <v>455644.86259355</v>
       </c>
       <c r="R68" s="1">
-        <v>11972785.789999999</v>
+        <v>13877989.750237687</v>
       </c>
       <c r="S68" s="1">
         <v>866499.98826533742</v>
@@ -6640,7 +6636,7 @@
         <v>741761.47744071996</v>
       </c>
       <c r="K69" s="1">
-        <v>552342.78</v>
+        <v>552416.69781284651</v>
       </c>
       <c r="L69" s="1">
         <v>30050557.612605866</v>
@@ -6661,7 +6657,7 @@
         <v>461805.94105485</v>
       </c>
       <c r="R69" s="1">
-        <v>11975299.42</v>
+        <v>13880903.371926771</v>
       </c>
       <c r="S69" s="1">
         <v>869908.38972472551</v>
@@ -6726,7 +6722,7 @@
         <v>737457.48933824</v>
       </c>
       <c r="K70" s="1">
-        <v>560220.1</v>
+        <v>560342.1277945406</v>
       </c>
       <c r="L70" s="1">
         <v>30695647.162182089</v>
@@ -6747,7 +6743,7 @@
         <v>470193.99712362001</v>
       </c>
       <c r="R70" s="1">
-        <v>12137688.380000001</v>
+        <v>14069132.934493141</v>
       </c>
       <c r="S70" s="1">
         <v>873559.08403702581</v>
@@ -6812,7 +6808,7 @@
         <v>742685.22420862003</v>
       </c>
       <c r="K71" s="1">
-        <v>561396.53</v>
+        <v>559716.09188914543</v>
       </c>
       <c r="L71" s="1">
         <v>31097580.59461854</v>
@@ -6833,7 +6829,7 @@
         <v>476818.86266296002</v>
       </c>
       <c r="R71" s="1">
-        <v>12205410.130000001</v>
+        <v>14147631.111394182</v>
       </c>
       <c r="S71" s="1">
         <v>871731.69919105899</v>
@@ -6898,7 +6894,7 @@
         <v>736830.15378312999</v>
       </c>
       <c r="K72" s="1">
-        <v>559074.99</v>
+        <v>560625.92048384144</v>
       </c>
       <c r="L72" s="1">
         <v>31532630.43853119</v>
@@ -6919,7 +6915,7 @@
         <v>482747.76864353003</v>
       </c>
       <c r="R72" s="1">
-        <v>12234870.189999999</v>
+        <v>14181779.081861349</v>
       </c>
       <c r="S72" s="1">
         <v>882913.46437223419</v>
@@ -6984,7 +6980,7 @@
         <v>742685.26106193999</v>
       </c>
       <c r="K73" s="1">
-        <v>558946.32999999996</v>
+        <v>558801.64877917583</v>
       </c>
       <c r="L73" s="1">
         <v>31998619.176453114</v>
@@ -7005,7 +7001,7 @@
         <v>487486.24439953995</v>
       </c>
       <c r="R73" s="1">
-        <v>12316105.640000001</v>
+        <v>14275941.363715477</v>
       </c>
       <c r="S73" s="1">
         <v>886028.2078166029</v>
@@ -7070,7 +7066,7 @@
         <v>748000.11716905003</v>
       </c>
       <c r="K74" s="1">
-        <v>561813.49</v>
+        <v>562817.04615272523</v>
       </c>
       <c r="L74" s="1">
         <v>32328694.532481011</v>
@@ -7091,7 +7087,7 @@
         <v>494286.65725309</v>
       </c>
       <c r="R74" s="1">
-        <v>12311415.939999999</v>
+        <v>14270505.39837384</v>
       </c>
       <c r="S74" s="1">
         <v>878001.32472443336</v>
@@ -7156,7 +7152,7 @@
         <v>746745.39077885996</v>
       </c>
       <c r="K75" s="1">
-        <v>562990.39</v>
+        <v>559562.27471337246</v>
       </c>
       <c r="L75" s="1">
         <v>32795590.569347434</v>
@@ -7177,7 +7173,7 @@
         <v>498756.97704818001</v>
       </c>
       <c r="R75" s="1">
-        <v>12589865.67</v>
+        <v>14593264.24134906</v>
       </c>
       <c r="S75" s="1">
         <v>881586.04402315104</v>
@@ -7242,7 +7238,7 @@
         <v>747581.86889677006</v>
       </c>
       <c r="K76" s="1">
-        <v>539934.27</v>
+        <v>540849.64619473077</v>
       </c>
       <c r="L76" s="1">
         <v>32980316.634457991</v>
@@ -7263,7 +7259,7 @@
         <v>502463.64743030001</v>
       </c>
       <c r="R76" s="1">
-        <v>12466691.99</v>
+        <v>14450490.191836016</v>
       </c>
       <c r="S76" s="1">
         <v>882807.12003215076</v>
@@ -7328,7 +7324,7 @@
         <v>749533.61124746001</v>
       </c>
       <c r="K77" s="1">
-        <v>538264.26</v>
+        <v>538803.87775695242</v>
       </c>
       <c r="L77" s="1">
         <v>33030671.725880675</v>
@@ -7349,7 +7345,7 @@
         <v>505748.37199040997</v>
       </c>
       <c r="R77" s="1">
-        <v>12410281.74</v>
+        <v>14385103.502538336</v>
       </c>
       <c r="S77" s="1">
         <v>882501.92792386026</v>

</xml_diff>